<commit_message>
Negative number visiblity changes in template
</commit_message>
<xml_diff>
--- a/src/Input/AppartementInfo.xlsx
+++ b/src/Input/AppartementInfo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InvGen\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\invoice-generator\src\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C91B70-DD09-438A-B1E5-1CA84A55CBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5A0A20-CCF5-4F81-9B12-90B7C8AF3CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD773AE9-4335-4BE7-A63B-9F3DEDF18284}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>3104</v>
       </c>
       <c r="E3">
-        <v>-8000</v>
+        <v>-80000</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>